<commit_message>
edit poc to wait for navigation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -117,8 +117,8 @@
     </font>
     <font>
       <color indexed="8"/>
-      <sz val="10"/>
-      <name val="Helvetica Neue"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -297,7 +297,7 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>

</xml_diff>